<commit_message>
test import en suspens
</commit_message>
<xml_diff>
--- a/Tests/test_recap_group_5-2.xlsx
+++ b/Tests/test_recap_group_5-2.xlsx
@@ -62,9 +62,6 @@
     <t>post_filtering</t>
   </si>
   <si>
-    <t>en suspens car besoin de mettre en place une architecture de test</t>
-  </si>
-  <si>
     <t>l'url est bien celle attendue</t>
   </si>
   <si>
@@ -90,6 +87,10 @@
   </si>
   <si>
     <t>identique à post_EN</t>
+  </si>
+  <si>
+    <t>en suspens car besoin de mettre en place une architecture de test
+attention le filepath fournit doit pointer vers les données du groupe 4</t>
   </si>
 </sst>
 </file>
@@ -185,7 +186,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -200,6 +200,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,7 +487,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +534,7 @@
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -540,146 +543,146 @@
       <c r="C3" s="9">
         <v>43116</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>15</v>
+      <c r="F3" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="14"/>
       <c r="C4" s="9">
         <v>43116</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="14"/>
       <c r="C5" s="9">
         <v>43116</v>
       </c>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="D6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="12"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="D6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="F7" s="12"/>
+      <c r="A7" s="14"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="9">
         <v>43117</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
       <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="9">
         <v>43117</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>19</v>
+      <c r="D11" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="D12" s="11"/>
       <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="D13" s="11"/>
       <c r="E13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="9">
         <v>43117</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>19</v>
+      <c r="D14" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="12"/>
+      <c r="D15" s="11"/>
       <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="11"/>
       <c r="E16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>

</xml_diff>